<commit_message>
distribution add information div
</commit_message>
<xml_diff>
--- a/public/Capacity Estimates Data.xlsx
+++ b/public/Capacity Estimates Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moyuzhanglaptop/前端/my_irp/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A5D1D3-50F7-904B-90E2-76DCF91FF224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0525DD0F-1CD1-574F-9E43-C6D7869C2CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6560" yWindow="-19140" windowWidth="24460" windowHeight="15840" xr2:uid="{17BA39F0-B877-F046-886A-9FDF553D753D}"/>
   </bookViews>
@@ -4266,10 +4266,10 @@
   <dimension ref="A1:BF767"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B760" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BF1" sqref="BF1"/>
+      <selection pane="bottomRight" activeCell="A768" sqref="A768:XFD768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -63259,12 +63259,8 @@
       </c>
     </row>
     <row r="767" spans="1:58">
-      <c r="E767" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F767" s="1" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="E767" s="1"/>
+      <c r="F767" s="1"/>
       <c r="AG767"/>
     </row>
   </sheetData>

</xml_diff>